<commit_message>
Updated Query for Slot.jsp
</commit_message>
<xml_diff>
--- a/src/data/output/workbook.xlsx
+++ b/src/data/output/workbook.xlsx
@@ -120,6 +120,16 @@
 [L]</t>
   </si>
   <si>
+    <t>CT513</t>
+  </si>
+  <si>
+    <t>Detection and Estimation Theory</t>
+  </si>
+  <si>
+    <t>6
+[L]</t>
+  </si>
+  <si>
     <t>IT543</t>
   </si>
   <si>
@@ -130,16 +140,6 @@
 [L]</t>
   </si>
   <si>
-    <t>CT513</t>
-  </si>
-  <si>
-    <t>Detection and Estimation Theory</t>
-  </si>
-  <si>
-    <t>6
-[L]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 14:00 - 16:00 </t>
   </si>
   <si>
@@ -255,6 +255,16 @@
 [R]</t>
   </si>
   <si>
+    <t>CS304</t>
+  </si>
+  <si>
+    <t>Introduction to Nonlinear Science</t>
+  </si>
+  <si>
+    <t>48
+[L]</t>
+  </si>
+  <si>
     <t>EL312</t>
   </si>
   <si>
@@ -265,16 +275,6 @@
 [L]</t>
   </si>
   <si>
-    <t>CS304</t>
-  </si>
-  <si>
-    <t>Introduction to Nonlinear Science</t>
-  </si>
-  <si>
-    <t>48
-[L]</t>
-  </si>
-  <si>
     <t>IT617</t>
   </si>
   <si>
@@ -329,6 +329,12 @@
 [L]</t>
   </si>
   <si>
+    <t>CT512</t>
+  </si>
+  <si>
+    <t>Information Theory and Coding</t>
+  </si>
+  <si>
     <t>IT410</t>
   </si>
   <si>
@@ -339,10 +345,14 @@
 [R]</t>
   </si>
   <si>
-    <t>CT512</t>
-  </si>
-  <si>
-    <t>Information Theory and Coding</t>
+    <t>IT415</t>
+  </si>
+  <si>
+    <t>Software Testing and Quality Analysis</t>
+  </si>
+  <si>
+    <t>5
+[R]</t>
   </si>
   <si>
     <t>CS302</t>
@@ -365,16 +375,6 @@
 [L]</t>
   </si>
   <si>
-    <t>IT415</t>
-  </si>
-  <si>
-    <t>Software Testing and Quality Analysis</t>
-  </si>
-  <si>
-    <t>5
-[R]</t>
-  </si>
-  <si>
     <t>IT694</t>
   </si>
   <si>
@@ -389,12 +389,6 @@
 [L]</t>
   </si>
   <si>
-    <t>EL520</t>
-  </si>
-  <si>
-    <t>Digital System Design using Verilog</t>
-  </si>
-  <si>
     <t>SC522</t>
   </si>
   <si>
@@ -405,6 +399,12 @@
 [L]</t>
   </si>
   <si>
+    <t>EL520</t>
+  </si>
+  <si>
+    <t>Digital System Design using Verilog</t>
+  </si>
+  <si>
     <t>CS201</t>
   </si>
   <si>
@@ -415,6 +415,30 @@
 [R]</t>
   </si>
   <si>
+    <t>IT325</t>
+  </si>
+  <si>
+    <t>Introduction to Cryptology</t>
+  </si>
+  <si>
+    <t>94
+[L]</t>
+  </si>
+  <si>
+    <t>18
+[L]</t>
+  </si>
+  <si>
+    <t>IT468</t>
+  </si>
+  <si>
+    <t>Natural Computing</t>
+  </si>
+  <si>
+    <t>38
+[L]</t>
+  </si>
+  <si>
     <t>IT422</t>
   </si>
   <si>
@@ -427,30 +451,6 @@
   <si>
     <t>58
 [R]</t>
-  </si>
-  <si>
-    <t>IT468</t>
-  </si>
-  <si>
-    <t>Natural Computing</t>
-  </si>
-  <si>
-    <t>38
-[L]</t>
-  </si>
-  <si>
-    <t>IT325</t>
-  </si>
-  <si>
-    <t>Introduction to Cryptology</t>
-  </si>
-  <si>
-    <t>94
-[L]</t>
-  </si>
-  <si>
-    <t>18
-[L]</t>
   </si>
   <si>
     <t>ES662</t>
@@ -1531,7 +1531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="true"/>
@@ -1868,6 +1868,10 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="40" borderId="22" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="centerContinuous" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="56" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true">
@@ -2329,10 +2333,9 @@
       <c r="N18" t="s" s="9">
         <v>33</v>
       </c>
-      <c r="S18" t="s" s="9">
+      <c r="T18" t="s" s="52">
         <v>34</v>
       </c>
-      <c r="T18" s="38"/>
       <c r="V18" s="27"/>
       <c r="AC18" s="38"/>
       <c r="AE18" t="s" s="50">
@@ -2357,9 +2360,10 @@
       <c r="N19" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="T19" t="s" s="52">
+      <c r="S19" t="s" s="9">
         <v>37</v>
       </c>
+      <c r="T19" s="38"/>
       <c r="V19" s="27"/>
       <c r="AC19" s="38"/>
       <c r="AE19" s="27"/>
@@ -2669,7 +2673,7 @@
       <c r="AF26" t="s" s="3">
         <v>74</v>
       </c>
-      <c r="AI26" t="s" s="3">
+      <c r="AH26" t="s" s="3">
         <v>75</v>
       </c>
       <c r="AL26" s="38"/>
@@ -2689,7 +2693,7 @@
       <c r="AF27" t="s" s="3">
         <v>77</v>
       </c>
-      <c r="AH27" t="s" s="3">
+      <c r="AI27" t="s" s="3">
         <v>78</v>
       </c>
       <c r="AL27" s="38"/>
@@ -2817,24 +2821,24 @@
       <c r="R32" s="26"/>
       <c r="S32" s="26"/>
       <c r="T32" s="36"/>
-      <c r="V32" t="s" s="114">
+      <c r="V32" t="s" s="115">
         <v>38</v>
       </c>
       <c r="W32" s="26"/>
       <c r="X32" s="26"/>
-      <c r="Y32" t="s" s="115">
+      <c r="Y32" t="s" s="116">
         <v>1</v>
       </c>
       <c r="Z32" s="26"/>
       <c r="AA32" s="26"/>
       <c r="AB32" s="26"/>
       <c r="AC32" s="36"/>
-      <c r="AE32" t="s" s="119">
+      <c r="AE32" t="s" s="120">
         <v>39</v>
       </c>
       <c r="AF32" s="26"/>
       <c r="AG32" s="26"/>
-      <c r="AH32" t="s" s="118">
+      <c r="AH32" t="s" s="119">
         <v>1</v>
       </c>
       <c r="AI32" s="26"/>
@@ -2968,8 +2972,14 @@
       <c r="AF35" t="s" s="3">
         <v>101</v>
       </c>
+      <c r="AH35" t="s" s="3">
+        <v>6</v>
+      </c>
       <c r="AI35" t="s" s="3">
         <v>102</v>
+      </c>
+      <c r="AJ35" t="s" s="3">
+        <v>7</v>
       </c>
       <c r="AL35" s="38"/>
     </row>
@@ -2996,7 +3006,7 @@
       <c r="AF36" t="s" s="3">
         <v>104</v>
       </c>
-      <c r="AJ36" t="s" s="3">
+      <c r="AI36" t="s" s="3">
         <v>105</v>
       </c>
       <c r="AL36" s="38"/>
@@ -3016,14 +3026,8 @@
       <c r="AF37" t="s" s="3">
         <v>107</v>
       </c>
-      <c r="AH37" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="AI37" t="s" s="3">
+      <c r="AJ37" t="s" s="3">
         <v>108</v>
-      </c>
-      <c r="AJ37" t="s" s="3">
-        <v>7</v>
       </c>
       <c r="AL37" s="38"/>
     </row>
@@ -3076,9 +3080,10 @@
       <c r="N39" t="s" s="9">
         <v>96</v>
       </c>
-      <c r="T39" t="s" s="52">
-        <v>97</v>
-      </c>
+      <c r="S39" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="T39" s="38"/>
       <c r="V39" s="27"/>
       <c r="AC39" s="38"/>
       <c r="AE39" t="s" s="50">
@@ -3088,7 +3093,7 @@
         <v>114</v>
       </c>
       <c r="AH39" t="s" s="9">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="AL39" s="38"/>
     </row>
@@ -3104,19 +3109,19 @@
       <c r="J40" s="41"/>
       <c r="K40" s="43"/>
       <c r="M40" t="s" s="89">
+        <v>97</v>
+      </c>
+      <c r="N40" t="s" s="90">
         <v>98</v>
-      </c>
-      <c r="N40" t="s" s="90">
-        <v>99</v>
       </c>
       <c r="O40" s="41"/>
       <c r="P40" s="41"/>
       <c r="Q40" s="41"/>
       <c r="R40" s="41"/>
-      <c r="S40" t="s" s="90">
-        <v>49</v>
-      </c>
-      <c r="T40" s="43"/>
+      <c r="S40" s="41"/>
+      <c r="T40" t="s" s="112">
+        <v>99</v>
+      </c>
       <c r="V40" s="40"/>
       <c r="W40" s="41"/>
       <c r="X40" s="41"/>
@@ -3126,14 +3131,14 @@
       <c r="AB40" s="41"/>
       <c r="AC40" s="43"/>
       <c r="AE40" t="s" s="89">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF40" t="s" s="90">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AG40" s="41"/>
       <c r="AH40" t="s" s="90">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="AI40" s="41"/>
       <c r="AJ40" s="41"/>
@@ -3145,48 +3150,48 @@
         <v>17</v>
       </c>
       <c r="C42" s="24"/>
-      <c r="D42" t="s" s="128">
+      <c r="D42" t="s" s="129">
         <v>0</v>
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
-      <c r="G42" t="s" s="131">
+      <c r="G42" t="s" s="132">
         <v>1</v>
       </c>
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
       <c r="J42" s="26"/>
       <c r="K42" s="36"/>
-      <c r="M42" t="s" s="137">
+      <c r="M42" t="s" s="138">
         <v>18</v>
       </c>
       <c r="N42" s="26"/>
       <c r="O42" s="26"/>
-      <c r="P42" t="s" s="138">
+      <c r="P42" t="s" s="139">
         <v>1</v>
       </c>
       <c r="Q42" s="26"/>
       <c r="R42" s="26"/>
       <c r="S42" s="26"/>
       <c r="T42" s="36"/>
-      <c r="V42" t="s" s="142">
+      <c r="V42" t="s" s="143">
         <v>38</v>
       </c>
       <c r="W42" s="26"/>
       <c r="X42" s="26"/>
-      <c r="Y42" t="s" s="141">
+      <c r="Y42" t="s" s="142">
         <v>1</v>
       </c>
       <c r="Z42" s="26"/>
       <c r="AA42" s="26"/>
       <c r="AB42" s="26"/>
       <c r="AC42" s="36"/>
-      <c r="AE42" t="s" s="145">
+      <c r="AE42" t="s" s="146">
         <v>39</v>
       </c>
       <c r="AF42" s="26"/>
       <c r="AG42" s="26"/>
-      <c r="AH42" t="s" s="146">
+      <c r="AH42" t="s" s="147">
         <v>1</v>
       </c>
       <c r="AI42" s="26"/>
@@ -3264,7 +3269,7 @@
     </row>
     <row r="44">
       <c r="B44" s="23"/>
-      <c r="C44" t="s" s="129">
+      <c r="C44" t="s" s="130">
         <v>3</v>
       </c>
       <c r="D44" s="27"/>
@@ -3286,7 +3291,7 @@
     </row>
     <row r="45">
       <c r="B45" s="23"/>
-      <c r="C45" t="s" s="130">
+      <c r="C45" t="s" s="131">
         <v>10</v>
       </c>
       <c r="D45" s="27"/>
@@ -3371,7 +3376,7 @@
     </row>
     <row r="48">
       <c r="B48" s="23"/>
-      <c r="C48" t="s" s="132">
+      <c r="C48" t="s" s="133">
         <v>14</v>
       </c>
       <c r="D48" s="27"/>
@@ -3396,7 +3401,7 @@
     </row>
     <row r="49">
       <c r="B49" s="23"/>
-      <c r="C49" t="s" s="133">
+      <c r="C49" t="s" s="134">
         <v>53</v>
       </c>
       <c r="D49" s="27"/>
@@ -3418,7 +3423,7 @@
     </row>
     <row r="50">
       <c r="B50" s="23"/>
-      <c r="C50" t="s" s="134">
+      <c r="C50" t="s" s="135">
         <v>15</v>
       </c>
       <c r="D50" s="27"/>

</xml_diff>

<commit_message>
Just Displaying courses not in the slot
</commit_message>
<xml_diff>
--- a/src/data/output/workbook.xlsx
+++ b/src/data/output/workbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="143">
   <si>
     <t xml:space="preserve"> 08:30 - 10:30 </t>
   </si>
@@ -86,6 +86,16 @@
 [R]</t>
   </si>
   <si>
+    <t>IT478</t>
+  </si>
+  <si>
+    <t>Internet of Things</t>
+  </si>
+  <si>
+    <t>60
+[L]</t>
+  </si>
+  <si>
     <t>EL426</t>
   </si>
   <si>
@@ -96,16 +106,6 @@
 [L]</t>
   </si>
   <si>
-    <t>IT478</t>
-  </si>
-  <si>
-    <t>Internet of Things</t>
-  </si>
-  <si>
-    <t>60
-[L]</t>
-  </si>
-  <si>
     <t>IT618</t>
   </si>
   <si>
@@ -120,6 +120,16 @@
 [L]</t>
   </si>
   <si>
+    <t>IT543</t>
+  </si>
+  <si>
+    <t>Adv. Logic for Computer Science</t>
+  </si>
+  <si>
+    <t>15
+[L]</t>
+  </si>
+  <si>
     <t>CT513</t>
   </si>
   <si>
@@ -130,38 +140,22 @@
 [L]</t>
   </si>
   <si>
-    <t>IT543</t>
-  </si>
-  <si>
-    <t>Adv. Logic for Computer Science</t>
-  </si>
-  <si>
-    <t>15
-[L]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 14:00 - 16:00 </t>
   </si>
   <si>
     <t xml:space="preserve"> 16:30 - 18:30 </t>
   </si>
   <si>
-    <t>SC209</t>
-  </si>
-  <si>
-    <t>Environmental Studies</t>
+    <t>SC465</t>
+  </si>
+  <si>
+    <t>Analysis of Multi-Disciplinary Problems</t>
   </si>
   <si>
     <t>14
 [R]</t>
   </si>
   <si>
-    <t>SC465</t>
-  </si>
-  <si>
-    <t>Analysis of Multi-Disciplinary Problems</t>
-  </si>
-  <si>
     <t>IT523</t>
   </si>
   <si>
@@ -172,169 +166,173 @@
   </si>
   <si>
     <t>Introduction to Narratology</t>
+  </si>
+  <si>
+    <t>12
+[R]</t>
+  </si>
+  <si>
+    <t>SC215</t>
+  </si>
+  <si>
+    <t>Probability and Statistics</t>
+  </si>
+  <si>
+    <t>13
+[R]</t>
+  </si>
+  <si>
+    <t>MScICTARD-I</t>
+  </si>
+  <si>
+    <t>SC205</t>
+  </si>
+  <si>
+    <t>Discrete Mathematics</t>
+  </si>
+  <si>
+    <t>27
+[R]</t>
+  </si>
+  <si>
+    <t>IT314</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>65
+[L]</t>
+  </si>
+  <si>
+    <t>54
+[L]</t>
+  </si>
+  <si>
+    <t>IT664</t>
+  </si>
+  <si>
+    <t>Remote Sensing and GIS</t>
+  </si>
+  <si>
+    <t>4
+[L]</t>
+  </si>
+  <si>
+    <t>IT215</t>
+  </si>
+  <si>
+    <t>Systems Software</t>
+  </si>
+  <si>
+    <t>15
+[R]</t>
+  </si>
+  <si>
+    <t>HM501</t>
+  </si>
+  <si>
+    <t>Communications Skills</t>
+  </si>
+  <si>
+    <t>70
+[L]</t>
+  </si>
+  <si>
+    <t>IT205</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>26
+[R]</t>
+  </si>
+  <si>
+    <t>CS304</t>
+  </si>
+  <si>
+    <t>Introduction to Nonlinear Science</t>
+  </si>
+  <si>
+    <t>48
+[L]</t>
+  </si>
+  <si>
+    <t>EL312</t>
+  </si>
+  <si>
+    <t>Solid State Devices</t>
+  </si>
+  <si>
+    <t>40
+[L]</t>
+  </si>
+  <si>
+    <t>IT617</t>
+  </si>
+  <si>
+    <t>Operating Systems</t>
+  </si>
+  <si>
+    <t>50
+[L]</t>
+  </si>
+  <si>
+    <t>20
+[L]</t>
+  </si>
+  <si>
+    <t>43
+[L]</t>
+  </si>
+  <si>
+    <t>CT214</t>
+  </si>
+  <si>
+    <t>Analog and Digital Communication</t>
+  </si>
+  <si>
+    <t>SC332</t>
+  </si>
+  <si>
+    <t>Introduction to Quantum Mechanics</t>
+  </si>
+  <si>
+    <t>61
+[L]</t>
+  </si>
+  <si>
+    <t>CT314</t>
+  </si>
+  <si>
+    <t>Statistical Communication Theory (GE)</t>
+  </si>
+  <si>
+    <t>33
+[L]</t>
+  </si>
+  <si>
+    <t>IT616</t>
+  </si>
+  <si>
+    <t>Analysis &amp; Design of Algorithms</t>
+  </si>
+  <si>
+    <t>11
+[L]</t>
+  </si>
+  <si>
+    <t>CT512</t>
+  </si>
+  <si>
+    <t>Information Theory and Coding</t>
   </si>
   <si>
     <t>12
 [L]</t>
   </si>
   <si>
-    <t>SC215</t>
-  </si>
-  <si>
-    <t>Probability and Statistics</t>
-  </si>
-  <si>
-    <t>13
-[R]</t>
-  </si>
-  <si>
-    <t>MScICTARD-I</t>
-  </si>
-  <si>
-    <t>SC205</t>
-  </si>
-  <si>
-    <t>Discrete Mathematics</t>
-  </si>
-  <si>
-    <t>27
-[R]</t>
-  </si>
-  <si>
-    <t>IT314</t>
-  </si>
-  <si>
-    <t>Software Engineering</t>
-  </si>
-  <si>
-    <t>65
-[L]</t>
-  </si>
-  <si>
-    <t>54
-[L]</t>
-  </si>
-  <si>
-    <t>IT664</t>
-  </si>
-  <si>
-    <t>Remote Sensing and GIS</t>
-  </si>
-  <si>
-    <t>4
-[L]</t>
-  </si>
-  <si>
-    <t>IT215</t>
-  </si>
-  <si>
-    <t>Systems Software</t>
-  </si>
-  <si>
-    <t>15
-[R]</t>
-  </si>
-  <si>
-    <t>HM501</t>
-  </si>
-  <si>
-    <t>Communications Skills</t>
-  </si>
-  <si>
-    <t>70
-[L]</t>
-  </si>
-  <si>
-    <t>IT205</t>
-  </si>
-  <si>
-    <t>Data Structures</t>
-  </si>
-  <si>
-    <t>26
-[R]</t>
-  </si>
-  <si>
-    <t>CS304</t>
-  </si>
-  <si>
-    <t>Introduction to Nonlinear Science</t>
-  </si>
-  <si>
-    <t>48
-[L]</t>
-  </si>
-  <si>
-    <t>EL312</t>
-  </si>
-  <si>
-    <t>Solid State Devices</t>
-  </si>
-  <si>
-    <t>40
-[L]</t>
-  </si>
-  <si>
-    <t>IT617</t>
-  </si>
-  <si>
-    <t>Operating Systems</t>
-  </si>
-  <si>
-    <t>50
-[L]</t>
-  </si>
-  <si>
-    <t>20
-[L]</t>
-  </si>
-  <si>
-    <t>43
-[L]</t>
-  </si>
-  <si>
-    <t>CT214</t>
-  </si>
-  <si>
-    <t>Analog and Digital Communication</t>
-  </si>
-  <si>
-    <t>SC332</t>
-  </si>
-  <si>
-    <t>Introduction to Quantum Mechanics</t>
-  </si>
-  <si>
-    <t>61
-[L]</t>
-  </si>
-  <si>
-    <t>CT314</t>
-  </si>
-  <si>
-    <t>Statistical Communication Theory (GE)</t>
-  </si>
-  <si>
-    <t>33
-[L]</t>
-  </si>
-  <si>
-    <t>IT616</t>
-  </si>
-  <si>
-    <t>Analysis &amp; Design of Algorithms</t>
-  </si>
-  <si>
-    <t>11
-[L]</t>
-  </si>
-  <si>
-    <t>CT512</t>
-  </si>
-  <si>
-    <t>Information Theory and Coding</t>
-  </si>
-  <si>
     <t>IT410</t>
   </si>
   <si>
@@ -345,6 +343,16 @@
 [R]</t>
   </si>
   <si>
+    <t>CS302</t>
+  </si>
+  <si>
+    <t>Modeling and Simulation</t>
+  </si>
+  <si>
+    <t>55
+[R]</t>
+  </si>
+  <si>
     <t>IT415</t>
   </si>
   <si>
@@ -355,16 +363,6 @@
 [R]</t>
   </si>
   <si>
-    <t>CS302</t>
-  </si>
-  <si>
-    <t>Modeling and Simulation</t>
-  </si>
-  <si>
-    <t>55
-[R]</t>
-  </si>
-  <si>
     <t>SC431</t>
   </si>
   <si>
@@ -389,6 +387,12 @@
 [L]</t>
   </si>
   <si>
+    <t>EL520</t>
+  </si>
+  <si>
+    <t>Digital System Design using Verilog</t>
+  </si>
+  <si>
     <t>SC522</t>
   </si>
   <si>
@@ -399,12 +403,6 @@
 [L]</t>
   </si>
   <si>
-    <t>EL520</t>
-  </si>
-  <si>
-    <t>Digital System Design using Verilog</t>
-  </si>
-  <si>
     <t>CS201</t>
   </si>
   <si>
@@ -415,6 +413,34 @@
 [R]</t>
   </si>
   <si>
+    <t>IT422</t>
+  </si>
+  <si>
+    <t>Models of Computation</t>
+  </si>
+  <si>
+    <t>78
+[R]</t>
+  </si>
+  <si>
+    <t>58
+[R]</t>
+  </si>
+  <si>
+    <t>IT325</t>
+  </si>
+  <si>
+    <t>Introduction to Cryptology</t>
+  </si>
+  <si>
+    <t>94
+[L]</t>
+  </si>
+  <si>
+    <t>18
+[L]</t>
+  </si>
+  <si>
     <t>IT468</t>
   </si>
   <si>
@@ -425,44 +451,10 @@
 [L]</t>
   </si>
   <si>
-    <t>IT325</t>
-  </si>
-  <si>
-    <t>Introduction to Cryptology</t>
-  </si>
-  <si>
-    <t>94
-[L]</t>
-  </si>
-  <si>
-    <t>18
-[L]</t>
-  </si>
-  <si>
-    <t>IT422</t>
-  </si>
-  <si>
-    <t>Models of Computation</t>
-  </si>
-  <si>
-    <t>78
-[R]</t>
-  </si>
-  <si>
-    <t>58
-[R]</t>
-  </si>
-  <si>
     <t>ES662</t>
   </si>
   <si>
     <t>Systems Approach to Sustainable Development</t>
-  </si>
-  <si>
-    <t>EL516</t>
-  </si>
-  <si>
-    <t>Analog CMOS IC Design</t>
   </si>
   <si>
     <t>CT516</t>
@@ -473,6 +465,12 @@
   <si>
     <t>7
 [R]</t>
+  </si>
+  <si>
+    <t>EL516</t>
+  </si>
+  <si>
+    <t>Analog CMOS IC Design</t>
   </si>
   <si>
     <t>IT308</t>
@@ -2215,27 +2213,8 @@
       <c r="T14" s="38"/>
       <c r="V14" s="27"/>
       <c r="AC14" s="38"/>
-      <c r="AE14" t="s" s="31">
-        <v>40</v>
-      </c>
-      <c r="AF14" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH14" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="AI14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="AJ14" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="AK14" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="AL14" t="s" s="42">
-        <v>42</v>
-      </c>
+      <c r="AE14" s="27"/>
+      <c r="AL14" s="38"/>
     </row>
     <row r="15">
       <c r="B15" s="23"/>
@@ -2258,17 +2237,17 @@
       <c r="N15" t="s" s="3">
         <v>23</v>
       </c>
-      <c r="Q15" t="s" s="3">
+      <c r="R15" t="s" s="3">
         <v>24</v>
       </c>
       <c r="T15" s="38"/>
       <c r="V15" s="27"/>
       <c r="AC15" s="38"/>
       <c r="AE15" t="s" s="33">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AF15" t="s" s="3">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AH15" t="s" s="3">
         <v>42</v>
@@ -2286,7 +2265,7 @@
       <c r="N16" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="R16" t="s" s="3">
+      <c r="Q16" t="s" s="3">
         <v>27</v>
       </c>
       <c r="T16" s="38"/>
@@ -2333,18 +2312,19 @@
       <c r="N18" t="s" s="9">
         <v>33</v>
       </c>
-      <c r="T18" t="s" s="52">
+      <c r="S18" t="s" s="9">
         <v>34</v>
       </c>
+      <c r="T18" s="38"/>
       <c r="V18" s="27"/>
       <c r="AC18" s="38"/>
       <c r="AE18" t="s" s="50">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AF18" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="AI18" t="s" s="9">
+        <v>44</v>
+      </c>
+      <c r="AH18" t="s" s="9">
         <v>42</v>
       </c>
       <c r="AL18" s="38"/>
@@ -2360,10 +2340,9 @@
       <c r="N19" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="S19" t="s" s="9">
+      <c r="T19" t="s" s="52">
         <v>37</v>
       </c>
-      <c r="T19" s="38"/>
       <c r="V19" s="27"/>
       <c r="AC19" s="38"/>
       <c r="AE19" s="27"/>
@@ -2399,17 +2378,17 @@
       <c r="AB20" s="41"/>
       <c r="AC20" s="43"/>
       <c r="AE20" t="s" s="61">
+        <v>45</v>
+      </c>
+      <c r="AF20" t="s" s="62">
+        <v>46</v>
+      </c>
+      <c r="AG20" s="41"/>
+      <c r="AH20" t="s" s="62">
         <v>47</v>
       </c>
-      <c r="AF20" t="s" s="62">
-        <v>48</v>
-      </c>
-      <c r="AG20" s="41"/>
-      <c r="AH20" s="41"/>
       <c r="AI20" s="41"/>
-      <c r="AJ20" t="s" s="62">
-        <v>49</v>
-      </c>
+      <c r="AJ20" s="41"/>
       <c r="AK20" s="41"/>
       <c r="AL20" s="43"/>
     </row>
@@ -2543,10 +2522,10 @@
       <c r="D24" s="27"/>
       <c r="K24" s="38"/>
       <c r="M24" t="s" s="47">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N24" t="s" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P24" t="s" s="1">
         <v>6</v>
@@ -2561,15 +2540,15 @@
         <v>7</v>
       </c>
       <c r="T24" t="s" s="51">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V24" s="27"/>
       <c r="AC24" s="38"/>
       <c r="AE24" t="s" s="47">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AF24" t="s" s="1">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AH24" t="s" s="1">
         <v>6</v>
@@ -2584,7 +2563,7 @@
         <v>7</v>
       </c>
       <c r="AL24" t="s" s="51">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25">
@@ -2593,10 +2572,10 @@
         <v>3</v>
       </c>
       <c r="D25" t="s" s="31">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>6</v>
@@ -2611,15 +2590,15 @@
         <v>7</v>
       </c>
       <c r="K25" t="s" s="42">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M25" s="27"/>
       <c r="T25" s="38"/>
       <c r="V25" t="s" s="31">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Y25" t="s" s="2">
         <v>6</v>
@@ -2634,7 +2613,7 @@
         <v>7</v>
       </c>
       <c r="AC25" t="s" s="42">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AE25" s="27"/>
       <c r="AL25" s="38"/>
@@ -2647,34 +2626,34 @@
       <c r="D26" s="27"/>
       <c r="K26" s="38"/>
       <c r="M26" t="s" s="33">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N26" t="s" s="3">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="P26" t="s" s="3">
         <v>30</v>
       </c>
       <c r="Q26" t="s" s="3">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="R26" t="s" s="3">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S26" t="s" s="3">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T26" s="38"/>
       <c r="V26" s="27"/>
       <c r="AC26" s="38"/>
       <c r="AE26" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="AF26" t="s" s="3">
+        <v>72</v>
+      </c>
+      <c r="AH26" t="s" s="3">
         <v>73</v>
-      </c>
-      <c r="AF26" t="s" s="3">
-        <v>74</v>
-      </c>
-      <c r="AH26" t="s" s="3">
-        <v>75</v>
       </c>
       <c r="AL26" s="38"/>
     </row>
@@ -2688,13 +2667,13 @@
       <c r="V27" s="27"/>
       <c r="AC27" s="38"/>
       <c r="AE27" t="s" s="33">
+        <v>74</v>
+      </c>
+      <c r="AF27" t="s" s="3">
+        <v>75</v>
+      </c>
+      <c r="AI27" t="s" s="3">
         <v>76</v>
-      </c>
-      <c r="AF27" t="s" s="3">
-        <v>77</v>
-      </c>
-      <c r="AI27" t="s" s="3">
-        <v>78</v>
       </c>
       <c r="AL27" s="38"/>
     </row>
@@ -2710,37 +2689,37 @@
       <c r="V28" s="27"/>
       <c r="AC28" s="38"/>
       <c r="AE28" t="s" s="49">
+        <v>77</v>
+      </c>
+      <c r="AF28" t="s" s="5">
+        <v>78</v>
+      </c>
+      <c r="AH28" t="s" s="5">
         <v>79</v>
       </c>
-      <c r="AF28" t="s" s="5">
+      <c r="AI28" t="s" s="5">
         <v>80</v>
       </c>
-      <c r="AH28" t="s" s="5">
+      <c r="AJ28" t="s" s="5">
         <v>81</v>
-      </c>
-      <c r="AI28" t="s" s="5">
-        <v>82</v>
-      </c>
-      <c r="AJ28" t="s" s="5">
-        <v>83</v>
       </c>
       <c r="AL28" s="38"/>
     </row>
     <row r="29">
       <c r="B29" s="23"/>
       <c r="C29" t="s" s="78">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" s="27"/>
       <c r="K29" s="38"/>
       <c r="M29" t="s" s="84">
+        <v>59</v>
+      </c>
+      <c r="N29" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="S29" t="s" s="7">
         <v>61</v>
-      </c>
-      <c r="N29" t="s" s="7">
-        <v>62</v>
-      </c>
-      <c r="S29" t="s" s="7">
-        <v>63</v>
       </c>
       <c r="T29" s="38"/>
       <c r="V29" s="27"/>
@@ -2770,14 +2749,14 @@
       <c r="S30" s="41"/>
       <c r="T30" s="43"/>
       <c r="V30" t="s" s="89">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W30" t="s" s="90">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="X30" s="41"/>
       <c r="Y30" t="s" s="90">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Z30" s="41"/>
       <c r="AA30" s="41"/>
@@ -2922,10 +2901,10 @@
       <c r="D34" s="27"/>
       <c r="K34" s="38"/>
       <c r="M34" t="s" s="31">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>6</v>
@@ -2955,31 +2934,25 @@
       <c r="D35" s="27"/>
       <c r="K35" s="38"/>
       <c r="M35" t="s" s="33">
+        <v>84</v>
+      </c>
+      <c r="N35" t="s" s="3">
+        <v>85</v>
+      </c>
+      <c r="R35" t="s" s="3">
         <v>86</v>
-      </c>
-      <c r="N35" t="s" s="3">
-        <v>87</v>
-      </c>
-      <c r="R35" t="s" s="3">
-        <v>88</v>
       </c>
       <c r="T35" s="38"/>
       <c r="V35" s="27"/>
       <c r="AC35" s="38"/>
       <c r="AE35" t="s" s="33">
+        <v>99</v>
+      </c>
+      <c r="AF35" t="s" s="3">
         <v>100</v>
       </c>
-      <c r="AF35" t="s" s="3">
+      <c r="AI35" t="s" s="3">
         <v>101</v>
-      </c>
-      <c r="AH35" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="AI35" t="s" s="3">
-        <v>102</v>
-      </c>
-      <c r="AJ35" t="s" s="3">
-        <v>7</v>
       </c>
       <c r="AL35" s="38"/>
     </row>
@@ -2989,25 +2962,31 @@
       <c r="D36" s="27"/>
       <c r="K36" s="38"/>
       <c r="M36" t="s" s="33">
+        <v>87</v>
+      </c>
+      <c r="N36" t="s" s="3">
+        <v>88</v>
+      </c>
+      <c r="Q36" t="s" s="3">
         <v>89</v>
-      </c>
-      <c r="N36" t="s" s="3">
-        <v>90</v>
-      </c>
-      <c r="Q36" t="s" s="3">
-        <v>91</v>
       </c>
       <c r="T36" s="38"/>
       <c r="V36" s="27"/>
       <c r="AC36" s="38"/>
       <c r="AE36" t="s" s="33">
+        <v>102</v>
+      </c>
+      <c r="AF36" t="s" s="3">
         <v>103</v>
       </c>
-      <c r="AF36" t="s" s="3">
+      <c r="AH36" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="AI36" t="s" s="3">
         <v>104</v>
       </c>
-      <c r="AI36" t="s" s="3">
-        <v>105</v>
+      <c r="AJ36" t="s" s="3">
+        <v>7</v>
       </c>
       <c r="AL36" s="38"/>
     </row>
@@ -3021,13 +3000,13 @@
       <c r="V37" s="27"/>
       <c r="AC37" s="38"/>
       <c r="AE37" t="s" s="33">
+        <v>105</v>
+      </c>
+      <c r="AF37" t="s" s="3">
         <v>106</v>
       </c>
-      <c r="AF37" t="s" s="3">
+      <c r="AJ37" t="s" s="3">
         <v>107</v>
-      </c>
-      <c r="AJ37" t="s" s="3">
-        <v>108</v>
       </c>
       <c r="AL37" s="38"/>
     </row>
@@ -3039,31 +3018,31 @@
       <c r="D38" s="27"/>
       <c r="K38" s="38"/>
       <c r="M38" t="s" s="49">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="N38" t="s" s="5">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P38" t="s" s="5">
         <v>30</v>
       </c>
       <c r="Q38" t="s" s="5">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T38" s="38"/>
       <c r="V38" s="27"/>
       <c r="AC38" s="38"/>
       <c r="AE38" t="s" s="49">
+        <v>108</v>
+      </c>
+      <c r="AF38" t="s" s="5">
         <v>109</v>
       </c>
-      <c r="AF38" t="s" s="5">
+      <c r="AH38" t="s" s="5">
         <v>110</v>
       </c>
-      <c r="AH38" t="s" s="5">
+      <c r="AI38" t="s" s="5">
         <v>111</v>
-      </c>
-      <c r="AI38" t="s" s="5">
-        <v>112</v>
       </c>
       <c r="AL38" s="38"/>
     </row>
@@ -3075,25 +3054,25 @@
       <c r="D39" s="27"/>
       <c r="K39" s="38"/>
       <c r="M39" t="s" s="50">
+        <v>93</v>
+      </c>
+      <c r="N39" t="s" s="9">
+        <v>94</v>
+      </c>
+      <c r="S39" t="s" s="9">
         <v>95</v>
-      </c>
-      <c r="N39" t="s" s="9">
-        <v>96</v>
-      </c>
-      <c r="S39" t="s" s="9">
-        <v>49</v>
       </c>
       <c r="T39" s="38"/>
       <c r="V39" s="27"/>
       <c r="AC39" s="38"/>
       <c r="AE39" t="s" s="50">
+        <v>112</v>
+      </c>
+      <c r="AF39" t="s" s="9">
         <v>113</v>
       </c>
-      <c r="AF39" t="s" s="9">
-        <v>114</v>
-      </c>
       <c r="AH39" t="s" s="9">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="AL39" s="38"/>
     </row>
@@ -3109,10 +3088,10 @@
       <c r="J40" s="41"/>
       <c r="K40" s="43"/>
       <c r="M40" t="s" s="89">
+        <v>96</v>
+      </c>
+      <c r="N40" t="s" s="90">
         <v>97</v>
-      </c>
-      <c r="N40" t="s" s="90">
-        <v>98</v>
       </c>
       <c r="O40" s="41"/>
       <c r="P40" s="41"/>
@@ -3120,7 +3099,7 @@
       <c r="R40" s="41"/>
       <c r="S40" s="41"/>
       <c r="T40" t="s" s="112">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V40" s="40"/>
       <c r="W40" s="41"/>
@@ -3131,14 +3110,14 @@
       <c r="AB40" s="41"/>
       <c r="AC40" s="43"/>
       <c r="AE40" t="s" s="89">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="AF40" t="s" s="90">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AG40" s="41"/>
       <c r="AH40" t="s" s="90">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="AI40" s="41"/>
       <c r="AJ40" s="41"/>
@@ -3275,13 +3254,13 @@
       <c r="D44" s="27"/>
       <c r="K44" s="38"/>
       <c r="M44" t="s" s="31">
+        <v>117</v>
+      </c>
+      <c r="N44" t="s" s="2">
         <v>118</v>
       </c>
-      <c r="N44" t="s" s="2">
+      <c r="R44" t="s" s="2">
         <v>119</v>
-      </c>
-      <c r="R44" t="s" s="2">
-        <v>120</v>
       </c>
       <c r="T44" s="38"/>
       <c r="V44" s="27"/>
@@ -3297,9 +3276,12 @@
       <c r="D45" s="27"/>
       <c r="K45" s="38"/>
       <c r="M45" t="s" s="33">
+        <v>120</v>
+      </c>
+      <c r="N45" t="s" s="3">
         <v>121</v>
       </c>
-      <c r="N45" t="s" s="3">
+      <c r="P45" t="s" s="3">
         <v>122</v>
       </c>
       <c r="Q45" t="s" s="3">
@@ -3309,10 +3291,10 @@
       <c r="V45" s="27"/>
       <c r="AC45" s="38"/>
       <c r="AE45" t="s" s="33">
+        <v>138</v>
+      </c>
+      <c r="AF45" t="s" s="3">
         <v>139</v>
-      </c>
-      <c r="AF45" t="s" s="3">
-        <v>140</v>
       </c>
       <c r="AH45" t="s" s="3">
         <v>6</v>
@@ -3324,7 +3306,7 @@
         <v>8</v>
       </c>
       <c r="AK45" t="s" s="3">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AL45" s="38"/>
     </row>
@@ -3362,11 +3344,8 @@
       <c r="N47" t="s" s="3">
         <v>129</v>
       </c>
-      <c r="P47" t="s" s="3">
+      <c r="Q47" t="s" s="3">
         <v>130</v>
-      </c>
-      <c r="Q47" t="s" s="3">
-        <v>131</v>
       </c>
       <c r="T47" s="38"/>
       <c r="V47" s="27"/>
@@ -3386,34 +3365,34 @@
       <c r="V48" s="27"/>
       <c r="AC48" s="38"/>
       <c r="AE48" t="s" s="49">
+        <v>141</v>
+      </c>
+      <c r="AF48" t="s" s="5">
         <v>142</v>
-      </c>
-      <c r="AF48" t="s" s="5">
-        <v>143</v>
       </c>
       <c r="AH48" t="s" s="5">
         <v>30</v>
       </c>
       <c r="AI48" t="s" s="5">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AL48" s="38"/>
     </row>
     <row r="49">
       <c r="B49" s="23"/>
       <c r="C49" t="s" s="134">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D49" s="27"/>
       <c r="K49" s="38"/>
       <c r="M49" t="s" s="84">
+        <v>131</v>
+      </c>
+      <c r="N49" t="s" s="7">
         <v>132</v>
       </c>
-      <c r="N49" t="s" s="7">
-        <v>133</v>
-      </c>
       <c r="P49" t="s" s="7">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="T49" s="38"/>
       <c r="V49" s="27"/>
@@ -3429,13 +3408,13 @@
       <c r="D50" s="27"/>
       <c r="K50" s="38"/>
       <c r="M50" t="s" s="50">
+        <v>133</v>
+      </c>
+      <c r="N50" t="s" s="9">
         <v>134</v>
       </c>
-      <c r="N50" t="s" s="9">
+      <c r="P50" t="s" s="9">
         <v>135</v>
-      </c>
-      <c r="P50" t="s" s="9">
-        <v>52</v>
       </c>
       <c r="T50" s="38"/>
       <c r="V50" s="27"/>
@@ -3462,7 +3441,7 @@
       </c>
       <c r="O51" s="41"/>
       <c r="P51" t="s" s="90">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="Q51" s="41"/>
       <c r="R51" s="41"/>

</xml_diff>

<commit_message>
File Upload/Download + UI Improvement
</commit_message>
<xml_diff>
--- a/src/data/output/workbook.xlsx
+++ b/src/data/output/workbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="143">
   <si>
     <t xml:space="preserve"> 09:00 - 12:00 </t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t>Analog Circuits</t>
+  </si>
+  <si>
+    <t>FFF</t>
   </si>
   <si>
     <t>98
@@ -51,6 +54,16 @@
     <t>BTech-III</t>
   </si>
   <si>
+    <t>IT483</t>
+  </si>
+  <si>
+    <t>Computational Electromagnetics</t>
+  </si>
+  <si>
+    <t>1
+[L]</t>
+  </si>
+  <si>
     <t>MScIT-I</t>
   </si>
   <si>
@@ -73,6 +86,16 @@
 [R]</t>
   </si>
   <si>
+    <t>EL426</t>
+  </si>
+  <si>
+    <t>Digital System Architecture (GE)</t>
+  </si>
+  <si>
+    <t>42
+[L]</t>
+  </si>
+  <si>
     <t>IT478</t>
   </si>
   <si>
@@ -83,26 +106,6 @@
 [L]</t>
   </si>
   <si>
-    <t>IT483</t>
-  </si>
-  <si>
-    <t>Computational Electromagnetics</t>
-  </si>
-  <si>
-    <t>1
-[L]</t>
-  </si>
-  <si>
-    <t>EL426</t>
-  </si>
-  <si>
-    <t>Digital System Architecture (GE)</t>
-  </si>
-  <si>
-    <t>42
-[L]</t>
-  </si>
-  <si>
     <t>IT618</t>
   </si>
   <si>
@@ -117,6 +120,16 @@
 [L]</t>
   </si>
   <si>
+    <t>IT543</t>
+  </si>
+  <si>
+    <t>Adv. Logic for Computer Science</t>
+  </si>
+  <si>
+    <t>15
+[L]</t>
+  </si>
+  <si>
     <t>CT513</t>
   </si>
   <si>
@@ -373,16 +386,6 @@
 [L]</t>
   </si>
   <si>
-    <t>EL520</t>
-  </si>
-  <si>
-    <t>Digital System Design using Verilog</t>
-  </si>
-  <si>
-    <t>15
-[L]</t>
-  </si>
-  <si>
     <t>SC522</t>
   </si>
   <si>
@@ -393,6 +396,12 @@
 [L]</t>
   </si>
   <si>
+    <t>EL520</t>
+  </si>
+  <si>
+    <t>Digital System Design using Verilog</t>
+  </si>
+  <si>
     <t>CS201</t>
   </si>
   <si>
@@ -403,6 +412,30 @@
 [R]</t>
   </si>
   <si>
+    <t>IT325</t>
+  </si>
+  <si>
+    <t>Introduction to Cryptology</t>
+  </si>
+  <si>
+    <t>94
+[L]</t>
+  </si>
+  <si>
+    <t>18
+[L]</t>
+  </si>
+  <si>
+    <t>IT468</t>
+  </si>
+  <si>
+    <t>Natural Computing</t>
+  </si>
+  <si>
+    <t>38
+[L]</t>
+  </si>
+  <si>
     <t>IT422</t>
   </si>
   <si>
@@ -417,40 +450,10 @@
 [R]</t>
   </si>
   <si>
-    <t>IT325</t>
-  </si>
-  <si>
-    <t>Introduction to Cryptology</t>
-  </si>
-  <si>
-    <t>94
-[L]</t>
-  </si>
-  <si>
-    <t>18
-[L]</t>
-  </si>
-  <si>
-    <t>IT468</t>
-  </si>
-  <si>
-    <t>Natural Computing</t>
-  </si>
-  <si>
-    <t>38
-[L]</t>
-  </si>
-  <si>
     <t>ES662</t>
   </si>
   <si>
     <t>Systems Approach to Sustainable Development</t>
-  </si>
-  <si>
-    <t>EL516</t>
-  </si>
-  <si>
-    <t>Analog CMOS IC Design</t>
   </si>
   <si>
     <t>CT516</t>
@@ -461,6 +464,12 @@
   <si>
     <t>7
 [R]</t>
+  </si>
+  <si>
+    <t>EL516</t>
+  </si>
+  <si>
+    <t>Analog CMOS IC Design</t>
   </si>
   <si>
     <t>IT308</t>
@@ -1569,7 +1578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="true"/>
@@ -1641,19 +1650,23 @@
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="26" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="33" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="12" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="39" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="33" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1695,14 +1708,14 @@
       <alignment horizontal="centerContinuous" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="26" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="26" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="43" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1715,7 +1728,7 @@
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="47" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="56" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1768,10 +1781,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="40" borderId="22" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="centerContinuous" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="43" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
@@ -1939,10 +1948,6 @@
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="56" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="40" borderId="17" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="centerContinuous" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
@@ -2117,7 +2122,8 @@
   <cols>
     <col min="3" max="3" width="12.99609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.6328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="23.0078125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="30.2421875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.06640625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="4.37890625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="4.37890625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="4.37890625" customWidth="true" bestFit="true"/>
@@ -2125,6 +2131,7 @@
     <col min="11" max="11" width="4.37890625" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="6.69140625" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="43.28125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="4.06640625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="4.37890625" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="4.37890625" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="4.37890625" customWidth="true" bestFit="true"/>
@@ -2134,7 +2141,7 @@
   <sheetData>
     <row r="11">
       <c r="B11" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" t="s" s="24">
@@ -2148,19 +2155,19 @@
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
-      <c r="K11" s="34"/>
-      <c r="M11" t="s" s="43">
-        <v>14</v>
+      <c r="K11" s="36"/>
+      <c r="M11" t="s" s="44">
+        <v>18</v>
       </c>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
-      <c r="P11" t="s" s="45">
+      <c r="P11" t="s" s="46">
         <v>1</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
-      <c r="T11" s="34"/>
+      <c r="T11" s="36"/>
     </row>
     <row r="12">
       <c r="B12" s="22"/>
@@ -2178,7 +2185,7 @@
       <c r="J12" t="n">
         <v>103.0</v>
       </c>
-      <c r="K12" t="n" s="37">
+      <c r="K12" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M12" s="26"/>
@@ -2194,7 +2201,7 @@
       <c r="S12" t="n">
         <v>103.0</v>
       </c>
-      <c r="T12" t="n" s="37">
+      <c r="T12" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
@@ -2204,27 +2211,30 @@
         <v>2</v>
       </c>
       <c r="D13" s="26"/>
-      <c r="K13" s="37"/>
-      <c r="M13" t="s" s="44">
-        <v>15</v>
+      <c r="K13" s="38"/>
+      <c r="M13" t="s" s="45">
+        <v>19</v>
       </c>
       <c r="N13" t="s" s="1">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="O13" t="s" s="1">
+        <v>6</v>
       </c>
       <c r="P13" t="s" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q13" t="s" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R13" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="S13" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="S13" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="T13" t="s" s="50">
-        <v>17</v>
+      <c r="T13" t="s" s="51">
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -2238,151 +2248,180 @@
       <c r="E14" t="s" s="2">
         <v>5</v>
       </c>
+      <c r="F14" t="s" s="2">
+        <v>6</v>
+      </c>
       <c r="G14" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I14" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="J14" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J14" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="K14" t="s" s="39">
-        <v>9</v>
+      <c r="K14" t="s" s="40">
+        <v>10</v>
       </c>
       <c r="M14" s="26"/>
-      <c r="T14" s="37"/>
+      <c r="T14" s="38"/>
     </row>
     <row r="15">
       <c r="B15" s="22"/>
       <c r="C15" t="s" s="31">
-        <v>10</v>
-      </c>
-      <c r="D15" s="26"/>
-      <c r="K15" s="37"/>
-      <c r="M15" t="s" s="46">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="D15" t="s" s="32">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="K15" s="38"/>
+      <c r="M15" t="s" s="32">
+        <v>22</v>
       </c>
       <c r="N15" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="R15" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="T15" s="37"/>
+        <v>23</v>
+      </c>
+      <c r="O15" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q15" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="T15" s="38"/>
     </row>
     <row r="16">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="26"/>
-      <c r="K16" s="37"/>
-      <c r="M16" t="s" s="46">
-        <v>21</v>
+      <c r="K16" s="38"/>
+      <c r="M16" t="s" s="32">
+        <v>25</v>
       </c>
       <c r="N16" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="T16" t="s" s="51">
-        <v>23</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="O16" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="R16" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="T16" s="38"/>
     </row>
     <row r="17">
       <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="C17" t="s" s="33">
+        <v>15</v>
+      </c>
       <c r="D17" s="26"/>
-      <c r="K17" s="37"/>
-      <c r="M17" t="s" s="46">
-        <v>24</v>
-      </c>
-      <c r="N17" t="s" s="3">
-        <v>25</v>
-      </c>
-      <c r="Q17" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="T17" s="37"/>
+      <c r="K17" s="38"/>
+      <c r="M17" t="s" s="47">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="O17" t="s" s="5">
+        <v>6</v>
+      </c>
+      <c r="P17" t="s" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q17" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="T17" s="38"/>
     </row>
     <row r="18">
       <c r="B18" s="22"/>
-      <c r="C18" t="s" s="33">
-        <v>11</v>
+      <c r="C18" t="s" s="35">
+        <v>16</v>
       </c>
       <c r="D18" s="26"/>
-      <c r="K18" s="37"/>
-      <c r="M18" t="s" s="47">
-        <v>27</v>
-      </c>
-      <c r="N18" t="s" s="5">
-        <v>28</v>
-      </c>
-      <c r="P18" t="s" s="5">
-        <v>29</v>
-      </c>
-      <c r="Q18" t="s" s="5">
-        <v>30</v>
-      </c>
-      <c r="T18" s="37"/>
+      <c r="K18" s="38"/>
+      <c r="M18" t="s" s="48">
+        <v>32</v>
+      </c>
+      <c r="N18" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="O18" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="S18" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="T18" s="38"/>
     </row>
     <row r="19">
-      <c r="B19" s="32"/>
-      <c r="C19" t="s" s="35">
-        <v>12</v>
-      </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="40"/>
-      <c r="M19" t="s" s="48">
-        <v>31</v>
-      </c>
-      <c r="N19" t="s" s="49">
-        <v>32</v>
-      </c>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" t="s" s="49">
-        <v>33</v>
-      </c>
-      <c r="T19" s="40"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="41"/>
+      <c r="M19" t="s" s="49">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s" s="50">
+        <v>36</v>
+      </c>
+      <c r="O19" t="s" s="50">
+        <v>6</v>
+      </c>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" t="s" s="52">
+        <v>37</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C21" s="23"/>
-      <c r="D21" t="s" s="59">
+      <c r="D21" t="s" s="60">
         <v>0</v>
       </c>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
-      <c r="G21" t="s" s="62">
+      <c r="G21" t="s" s="63">
         <v>1</v>
       </c>
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
-      <c r="K21" s="34"/>
-      <c r="M21" t="s" s="67">
-        <v>14</v>
+      <c r="K21" s="36"/>
+      <c r="M21" t="s" s="68">
+        <v>18</v>
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
-      <c r="P21" t="s" s="68">
+      <c r="P21" t="s" s="69">
         <v>1</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
-      <c r="T21" s="34"/>
+      <c r="T21" s="36"/>
     </row>
     <row r="22">
       <c r="B22" s="22"/>
@@ -2400,7 +2439,7 @@
       <c r="J22" t="n">
         <v>103.0</v>
       </c>
-      <c r="K22" t="n" s="37">
+      <c r="K22" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M22" s="26"/>
@@ -2416,106 +2455,117 @@
       <c r="S22" t="n">
         <v>103.0</v>
       </c>
-      <c r="T22" t="n" s="37">
+      <c r="T22" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="22"/>
-      <c r="C23" t="s" s="60">
+      <c r="C23" t="s" s="61">
         <v>3</v>
       </c>
       <c r="D23" s="26"/>
-      <c r="K23" s="37"/>
+      <c r="K23" s="38"/>
       <c r="M23" t="s" s="30">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="O23" t="s" s="2">
+        <v>6</v>
       </c>
       <c r="P23" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q23" t="s" s="2">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="R23" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="S23" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="S23" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="T23" t="s" s="39">
-        <v>37</v>
+      <c r="T23" t="s" s="40">
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="22"/>
-      <c r="C24" t="s" s="61">
-        <v>10</v>
+      <c r="C24" t="s" s="62">
+        <v>11</v>
       </c>
       <c r="D24" s="26"/>
-      <c r="K24" s="37"/>
-      <c r="M24" t="s" s="46">
-        <v>38</v>
+      <c r="K24" s="38"/>
+      <c r="M24" t="s" s="32">
+        <v>42</v>
       </c>
       <c r="N24" t="s" s="3">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="O24" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="P24" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="T24" s="37"/>
+        <v>41</v>
+      </c>
+      <c r="T24" s="38"/>
     </row>
     <row r="25">
       <c r="B25" s="22"/>
-      <c r="C25" t="s" s="63">
-        <v>12</v>
+      <c r="C25" t="s" s="64">
+        <v>16</v>
       </c>
       <c r="D25" s="26"/>
-      <c r="K25" s="37"/>
-      <c r="M25" t="s" s="69">
-        <v>40</v>
+      <c r="K25" s="38"/>
+      <c r="M25" t="s" s="48">
+        <v>44</v>
       </c>
       <c r="N25" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="O25" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q25" t="s" s="9">
         <v>41</v>
       </c>
-      <c r="Q25" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="T25" s="37"/>
+      <c r="T25" s="38"/>
     </row>
     <row r="26">
-      <c r="B26" s="32"/>
-      <c r="C26" t="s" s="64">
-        <v>34</v>
-      </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="40"/>
+      <c r="B26" s="34"/>
+      <c r="C26" t="s" s="65">
+        <v>38</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="41"/>
       <c r="M26" t="s" s="70">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="N26" t="s" s="71">
-        <v>43</v>
-      </c>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
+        <v>47</v>
+      </c>
+      <c r="O26" t="s" s="71">
+        <v>6</v>
+      </c>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
       <c r="R26" t="s" s="71">
-        <v>44</v>
-      </c>
-      <c r="S26" s="38"/>
-      <c r="T26" s="40"/>
+        <v>48</v>
+      </c>
+      <c r="S26" s="39"/>
+      <c r="T26" s="41"/>
     </row>
     <row r="28">
       <c r="B28" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" t="s" s="79">
@@ -2529,9 +2579,9 @@
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
       <c r="J28" s="25"/>
-      <c r="K28" s="34"/>
+      <c r="K28" s="36"/>
       <c r="M28" t="s" s="87">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
@@ -2541,7 +2591,7 @@
       <c r="Q28" s="25"/>
       <c r="R28" s="25"/>
       <c r="S28" s="25"/>
-      <c r="T28" s="34"/>
+      <c r="T28" s="36"/>
     </row>
     <row r="29">
       <c r="B29" s="22"/>
@@ -2559,7 +2609,7 @@
       <c r="J29" t="n">
         <v>103.0</v>
       </c>
-      <c r="K29" t="n" s="37">
+      <c r="K29" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M29" s="26"/>
@@ -2575,7 +2625,7 @@
       <c r="S29" t="n">
         <v>103.0</v>
       </c>
-      <c r="T29" t="n" s="37">
+      <c r="T29" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
@@ -2585,27 +2635,30 @@
         <v>2</v>
       </c>
       <c r="D30" s="26"/>
-      <c r="K30" s="37"/>
-      <c r="M30" t="s" s="44">
-        <v>49</v>
+      <c r="K30" s="38"/>
+      <c r="M30" t="s" s="45">
+        <v>53</v>
       </c>
       <c r="N30" t="s" s="1">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="O30" t="s" s="1">
+        <v>6</v>
       </c>
       <c r="P30" t="s" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q30" t="s" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R30" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="S30" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="S30" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="T30" t="s" s="50">
-        <v>51</v>
+      <c r="T30" t="s" s="51">
+        <v>55</v>
       </c>
     </row>
     <row r="31">
@@ -2614,87 +2667,95 @@
         <v>3</v>
       </c>
       <c r="D31" t="s" s="30">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E31" t="s" s="2">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="F31" t="s" s="2">
+        <v>6</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I31" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="J31" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J31" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="K31" t="s" s="39">
-        <v>47</v>
+      <c r="K31" t="s" s="40">
+        <v>51</v>
       </c>
       <c r="M31" s="26"/>
-      <c r="T31" s="37"/>
+      <c r="T31" s="38"/>
     </row>
     <row r="32">
       <c r="B32" s="22"/>
       <c r="C32" t="s" s="83">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D32" s="26"/>
-      <c r="K32" s="37"/>
-      <c r="M32" t="s" s="46">
+      <c r="K32" s="38"/>
+      <c r="M32" t="s" s="32">
+        <v>56</v>
+      </c>
+      <c r="N32" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="O32" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="P32" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="Q32" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="R32" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="S32" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="T32" s="38"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="34"/>
+      <c r="C33" t="s" s="84">
         <v>52</v>
       </c>
-      <c r="N32" t="s" s="3">
-        <v>53</v>
-      </c>
-      <c r="P32" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="Q32" t="s" s="3">
-        <v>20</v>
-      </c>
-      <c r="R32" t="s" s="3">
-        <v>54</v>
-      </c>
-      <c r="S32" t="s" s="3">
-        <v>55</v>
-      </c>
-      <c r="T32" s="37"/>
-    </row>
-    <row r="33">
-      <c r="B33" s="32"/>
-      <c r="C33" t="s" s="84">
-        <v>48</v>
-      </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="40"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="41"/>
       <c r="M33" t="s" s="89">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="N33" t="s" s="90">
-        <v>57</v>
-      </c>
-      <c r="O33" s="38"/>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="38"/>
-      <c r="R33" s="38"/>
+        <v>61</v>
+      </c>
+      <c r="O33" t="s" s="90">
+        <v>6</v>
+      </c>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="39"/>
       <c r="S33" t="s" s="90">
-        <v>58</v>
-      </c>
-      <c r="T33" s="40"/>
+        <v>62</v>
+      </c>
+      <c r="T33" s="41"/>
     </row>
     <row r="35">
       <c r="B35" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" t="s" s="99">
@@ -2708,9 +2769,9 @@
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
       <c r="J35" s="25"/>
-      <c r="K35" s="34"/>
+      <c r="K35" s="36"/>
       <c r="M35" t="s" s="108">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
@@ -2720,7 +2781,7 @@
       <c r="Q35" s="25"/>
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
-      <c r="T35" s="34"/>
+      <c r="T35" s="36"/>
     </row>
     <row r="36">
       <c r="B36" s="22"/>
@@ -2738,7 +2799,7 @@
       <c r="J36" t="n">
         <v>103.0</v>
       </c>
-      <c r="K36" t="n" s="37">
+      <c r="K36" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M36" s="26"/>
@@ -2754,7 +2815,7 @@
       <c r="S36" t="n">
         <v>103.0</v>
       </c>
-      <c r="T36" t="n" s="37">
+      <c r="T36" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
@@ -2764,27 +2825,30 @@
         <v>2</v>
       </c>
       <c r="D37" s="26"/>
-      <c r="K37" s="37"/>
-      <c r="M37" t="s" s="44">
-        <v>65</v>
+      <c r="K37" s="38"/>
+      <c r="M37" t="s" s="45">
+        <v>69</v>
       </c>
       <c r="N37" t="s" s="1">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="O37" t="s" s="1">
+        <v>6</v>
       </c>
       <c r="P37" t="s" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q37" t="s" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R37" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="S37" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="S37" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="T37" t="s" s="50">
-        <v>67</v>
+      <c r="T37" t="s" s="51">
+        <v>71</v>
       </c>
     </row>
     <row r="38">
@@ -2793,118 +2857,132 @@
         <v>3</v>
       </c>
       <c r="D38" t="s" s="30">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s" s="2">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="F38" t="s" s="2">
+        <v>6</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I38" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="J38" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J38" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="K38" t="s" s="39">
-        <v>61</v>
+      <c r="K38" t="s" s="40">
+        <v>65</v>
       </c>
       <c r="M38" s="26"/>
-      <c r="T38" s="37"/>
+      <c r="T38" s="38"/>
     </row>
     <row r="39">
       <c r="B39" s="22"/>
       <c r="C39" t="s" s="103">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D39" s="26"/>
-      <c r="K39" s="37"/>
-      <c r="M39" t="s" s="46">
-        <v>68</v>
+      <c r="K39" s="38"/>
+      <c r="M39" t="s" s="32">
+        <v>72</v>
       </c>
       <c r="N39" t="s" s="3">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="O39" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="P39" t="s" s="3">
-        <v>70</v>
-      </c>
-      <c r="T39" s="37"/>
+        <v>74</v>
+      </c>
+      <c r="T39" s="38"/>
     </row>
     <row r="40">
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="26"/>
-      <c r="K40" s="37"/>
-      <c r="M40" t="s" s="46">
-        <v>71</v>
+      <c r="K40" s="38"/>
+      <c r="M40" t="s" s="32">
+        <v>75</v>
       </c>
       <c r="N40" t="s" s="3">
-        <v>72</v>
+        <v>76</v>
+      </c>
+      <c r="O40" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="Q40" t="s" s="3">
-        <v>73</v>
-      </c>
-      <c r="T40" s="37"/>
+        <v>77</v>
+      </c>
+      <c r="T40" s="38"/>
     </row>
     <row r="41">
       <c r="B41" s="22"/>
       <c r="C41" t="s" s="104">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D41" s="26"/>
-      <c r="K41" s="37"/>
+      <c r="K41" s="38"/>
       <c r="M41" t="s" s="47">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="N41" t="s" s="5">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="O41" t="s" s="5">
+        <v>6</v>
       </c>
       <c r="P41" t="s" s="5">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="Q41" t="s" s="5">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="R41" t="s" s="5">
-        <v>78</v>
-      </c>
-      <c r="T41" s="37"/>
+        <v>82</v>
+      </c>
+      <c r="T41" s="38"/>
     </row>
     <row r="42">
-      <c r="B42" s="32"/>
+      <c r="B42" s="34"/>
       <c r="C42" t="s" s="105">
-        <v>12</v>
-      </c>
-      <c r="D42" t="s" s="48">
-        <v>62</v>
-      </c>
-      <c r="E42" t="s" s="49">
-        <v>63</v>
-      </c>
-      <c r="F42" s="38"/>
-      <c r="G42" t="s" s="49">
-        <v>64</v>
-      </c>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="40"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="38"/>
-      <c r="P42" s="38"/>
-      <c r="Q42" s="38"/>
-      <c r="R42" s="38"/>
-      <c r="S42" s="38"/>
-      <c r="T42" s="40"/>
+        <v>16</v>
+      </c>
+      <c r="D42" t="s" s="49">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s" s="50">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s" s="50">
+        <v>6</v>
+      </c>
+      <c r="G42" t="s" s="50">
+        <v>68</v>
+      </c>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="41"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="39"/>
+      <c r="R42" s="39"/>
+      <c r="S42" s="39"/>
+      <c r="T42" s="41"/>
     </row>
     <row r="44">
       <c r="B44" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" t="s" s="117">
@@ -2918,19 +2996,19 @@
       <c r="H44" s="25"/>
       <c r="I44" s="25"/>
       <c r="J44" s="25"/>
-      <c r="K44" s="34"/>
-      <c r="M44" t="s" s="126">
-        <v>14</v>
+      <c r="K44" s="36"/>
+      <c r="M44" t="s" s="125">
+        <v>18</v>
       </c>
       <c r="N44" s="25"/>
       <c r="O44" s="25"/>
-      <c r="P44" t="s" s="127">
+      <c r="P44" t="s" s="126">
         <v>1</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
-      <c r="T44" s="34"/>
+      <c r="T44" s="36"/>
     </row>
     <row r="45">
       <c r="B45" s="22"/>
@@ -2948,7 +3026,7 @@
       <c r="J45" t="n">
         <v>103.0</v>
       </c>
-      <c r="K45" t="n" s="37">
+      <c r="K45" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M45" s="26"/>
@@ -2964,7 +3042,7 @@
       <c r="S45" t="n">
         <v>103.0</v>
       </c>
-      <c r="T45" t="n" s="37">
+      <c r="T45" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
@@ -2974,157 +3052,174 @@
         <v>3</v>
       </c>
       <c r="D46" s="26"/>
-      <c r="K46" s="37"/>
+      <c r="K46" s="38"/>
       <c r="M46" t="s" s="30">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="O46" t="s" s="2">
+        <v>6</v>
       </c>
       <c r="P46" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q46" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R46" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="S46" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="S46" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="T46" t="s" s="39">
-        <v>37</v>
+      <c r="T46" t="s" s="40">
+        <v>41</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="22"/>
       <c r="C47" t="s" s="119">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D47" s="26"/>
-      <c r="K47" s="37"/>
-      <c r="M47" t="s" s="46">
-        <v>81</v>
+      <c r="K47" s="38"/>
+      <c r="M47" t="s" s="32">
+        <v>85</v>
       </c>
       <c r="N47" t="s" s="3">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="O47" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="R47" t="s" s="3">
-        <v>83</v>
-      </c>
-      <c r="T47" s="37"/>
+        <v>87</v>
+      </c>
+      <c r="T47" s="38"/>
     </row>
     <row r="48">
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="26"/>
-      <c r="K48" s="37"/>
-      <c r="M48" t="s" s="46">
-        <v>84</v>
+      <c r="K48" s="38"/>
+      <c r="M48" t="s" s="32">
+        <v>88</v>
       </c>
       <c r="N48" t="s" s="3">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="O48" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="Q48" t="s" s="3">
-        <v>86</v>
-      </c>
-      <c r="T48" s="37"/>
+        <v>90</v>
+      </c>
+      <c r="T48" s="38"/>
     </row>
     <row r="49">
       <c r="B49" s="22"/>
       <c r="C49" t="s" s="121">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D49" s="26"/>
-      <c r="K49" s="37"/>
+      <c r="K49" s="38"/>
       <c r="M49" t="s" s="47">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="N49" t="s" s="5">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="O49" t="s" s="5">
+        <v>6</v>
       </c>
       <c r="P49" t="s" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q49" t="s" s="5">
-        <v>89</v>
-      </c>
-      <c r="T49" s="37"/>
+        <v>93</v>
+      </c>
+      <c r="T49" s="38"/>
     </row>
     <row r="50">
       <c r="B50" s="22"/>
       <c r="C50" t="s" s="122">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D50" s="26"/>
-      <c r="K50" s="37"/>
-      <c r="M50" t="s" s="69">
-        <v>90</v>
+      <c r="K50" s="38"/>
+      <c r="M50" t="s" s="48">
+        <v>94</v>
       </c>
       <c r="N50" t="s" s="9">
-        <v>91</v>
+        <v>95</v>
+      </c>
+      <c r="O50" t="s" s="9">
+        <v>6</v>
       </c>
       <c r="S50" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="T50" s="37"/>
+        <v>48</v>
+      </c>
+      <c r="T50" s="38"/>
     </row>
     <row r="51">
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
-      <c r="J51" s="38"/>
-      <c r="K51" s="40"/>
-      <c r="M51" t="s" s="48">
-        <v>92</v>
-      </c>
-      <c r="N51" t="s" s="49">
-        <v>93</v>
-      </c>
-      <c r="O51" s="38"/>
-      <c r="P51" s="38"/>
-      <c r="Q51" s="38"/>
-      <c r="R51" s="38"/>
-      <c r="S51" s="38"/>
-      <c r="T51" t="s" s="125">
-        <v>94</v>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="39"/>
+      <c r="H51" s="39"/>
+      <c r="I51" s="39"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="41"/>
+      <c r="M51" t="s" s="49">
+        <v>96</v>
+      </c>
+      <c r="N51" t="s" s="50">
+        <v>97</v>
+      </c>
+      <c r="O51" t="s" s="50">
+        <v>6</v>
+      </c>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="39"/>
+      <c r="R51" s="39"/>
+      <c r="S51" s="39"/>
+      <c r="T51" t="s" s="52">
+        <v>98</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C53" s="23"/>
-      <c r="D53" t="s" s="134">
+      <c r="D53" t="s" s="133">
         <v>0</v>
       </c>
       <c r="E53" s="25"/>
       <c r="F53" s="25"/>
-      <c r="G53" t="s" s="136">
+      <c r="G53" t="s" s="135">
         <v>1</v>
       </c>
       <c r="H53" s="25"/>
       <c r="I53" s="25"/>
       <c r="J53" s="25"/>
-      <c r="K53" s="34"/>
-      <c r="M53" t="s" s="141">
-        <v>14</v>
+      <c r="K53" s="36"/>
+      <c r="M53" t="s" s="140">
+        <v>18</v>
       </c>
       <c r="N53" s="25"/>
       <c r="O53" s="25"/>
-      <c r="P53" t="s" s="142">
+      <c r="P53" t="s" s="141">
         <v>1</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="25"/>
       <c r="S53" s="25"/>
-      <c r="T53" s="34"/>
+      <c r="T53" s="36"/>
     </row>
     <row r="54">
       <c r="B54" s="22"/>
@@ -3142,7 +3237,7 @@
       <c r="J54" t="n">
         <v>103.0</v>
       </c>
-      <c r="K54" t="n" s="37">
+      <c r="K54" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M54" s="26"/>
@@ -3158,160 +3253,177 @@
       <c r="S54" t="n">
         <v>103.0</v>
       </c>
-      <c r="T54" t="n" s="37">
+      <c r="T54" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="22"/>
-      <c r="C55" t="s" s="135">
-        <v>10</v>
+      <c r="C55" t="s" s="134">
+        <v>11</v>
       </c>
       <c r="D55" s="26"/>
-      <c r="K55" s="37"/>
-      <c r="M55" t="s" s="46">
-        <v>95</v>
+      <c r="K55" s="38"/>
+      <c r="M55" t="s" s="32">
+        <v>99</v>
       </c>
       <c r="N55" t="s" s="3">
-        <v>96</v>
+        <v>100</v>
+      </c>
+      <c r="O55" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="Q55" t="s" s="3">
-        <v>97</v>
-      </c>
-      <c r="T55" s="37"/>
+        <v>101</v>
+      </c>
+      <c r="T55" s="38"/>
     </row>
     <row r="56">
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
       <c r="D56" s="26"/>
-      <c r="K56" s="37"/>
-      <c r="M56" t="s" s="46">
-        <v>98</v>
+      <c r="K56" s="38"/>
+      <c r="M56" t="s" s="32">
+        <v>102</v>
       </c>
       <c r="N56" t="s" s="3">
-        <v>99</v>
+        <v>103</v>
+      </c>
+      <c r="O56" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="P56" t="s" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q56" t="s" s="3">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="R56" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="T56" s="37"/>
+        <v>8</v>
+      </c>
+      <c r="T56" s="38"/>
     </row>
     <row r="57">
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
       <c r="D57" s="26"/>
-      <c r="K57" s="37"/>
-      <c r="M57" t="s" s="46">
-        <v>101</v>
+      <c r="K57" s="38"/>
+      <c r="M57" t="s" s="32">
+        <v>105</v>
       </c>
       <c r="N57" t="s" s="3">
-        <v>102</v>
+        <v>106</v>
+      </c>
+      <c r="O57" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="R57" t="s" s="3">
-        <v>103</v>
-      </c>
-      <c r="T57" s="37"/>
+        <v>107</v>
+      </c>
+      <c r="T57" s="38"/>
     </row>
     <row r="58">
       <c r="B58" s="22"/>
-      <c r="C58" t="s" s="137">
-        <v>11</v>
+      <c r="C58" t="s" s="136">
+        <v>15</v>
       </c>
       <c r="D58" s="26"/>
-      <c r="K58" s="37"/>
+      <c r="K58" s="38"/>
       <c r="M58" t="s" s="47">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="N58" t="s" s="5">
-        <v>105</v>
+        <v>109</v>
+      </c>
+      <c r="O58" t="s" s="5">
+        <v>6</v>
       </c>
       <c r="P58" t="s" s="5">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="Q58" t="s" s="5">
-        <v>107</v>
-      </c>
-      <c r="T58" s="37"/>
+        <v>111</v>
+      </c>
+      <c r="T58" s="38"/>
     </row>
     <row r="59">
       <c r="B59" s="22"/>
-      <c r="C59" t="s" s="138">
-        <v>12</v>
+      <c r="C59" t="s" s="137">
+        <v>16</v>
       </c>
       <c r="D59" s="26"/>
-      <c r="K59" s="37"/>
-      <c r="M59" t="s" s="69">
-        <v>108</v>
+      <c r="K59" s="38"/>
+      <c r="M59" t="s" s="48">
+        <v>112</v>
       </c>
       <c r="N59" t="s" s="9">
-        <v>109</v>
+        <v>113</v>
+      </c>
+      <c r="O59" t="s" s="9">
+        <v>6</v>
       </c>
       <c r="P59" t="s" s="9">
-        <v>110</v>
-      </c>
-      <c r="T59" s="37"/>
+        <v>114</v>
+      </c>
+      <c r="T59" s="38"/>
     </row>
     <row r="60">
-      <c r="B60" s="32"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="38"/>
-      <c r="H60" s="38"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="38"/>
-      <c r="K60" s="40"/>
-      <c r="M60" t="s" s="48">
-        <v>111</v>
-      </c>
-      <c r="N60" t="s" s="49">
-        <v>112</v>
-      </c>
-      <c r="O60" s="38"/>
-      <c r="P60" t="s" s="49">
-        <v>113</v>
-      </c>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="38"/>
-      <c r="S60" s="38"/>
-      <c r="T60" s="40"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="41"/>
+      <c r="M60" t="s" s="49">
+        <v>115</v>
+      </c>
+      <c r="N60" t="s" s="50">
+        <v>116</v>
+      </c>
+      <c r="O60" t="s" s="50">
+        <v>6</v>
+      </c>
+      <c r="P60" t="s" s="50">
+        <v>34</v>
+      </c>
+      <c r="Q60" s="39"/>
+      <c r="R60" s="39"/>
+      <c r="S60" s="39"/>
+      <c r="T60" s="41"/>
     </row>
     <row r="62">
       <c r="B62" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C62" s="23"/>
-      <c r="D62" t="s" s="150">
+      <c r="D62" t="s" s="149">
         <v>0</v>
       </c>
       <c r="E62" s="25"/>
       <c r="F62" s="25"/>
-      <c r="G62" t="s" s="153">
+      <c r="G62" t="s" s="152">
         <v>1</v>
       </c>
       <c r="H62" s="25"/>
       <c r="I62" s="25"/>
       <c r="J62" s="25"/>
-      <c r="K62" s="34"/>
-      <c r="M62" t="s" s="158">
-        <v>14</v>
+      <c r="K62" s="36"/>
+      <c r="M62" t="s" s="157">
+        <v>18</v>
       </c>
       <c r="N62" s="25"/>
       <c r="O62" s="25"/>
-      <c r="P62" t="s" s="159">
+      <c r="P62" t="s" s="158">
         <v>1</v>
       </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="25"/>
       <c r="S62" s="25"/>
-      <c r="T62" s="34"/>
+      <c r="T62" s="36"/>
     </row>
     <row r="63">
       <c r="B63" s="22"/>
@@ -3329,7 +3441,7 @@
       <c r="J63" t="n">
         <v>103.0</v>
       </c>
-      <c r="K63" t="n" s="37">
+      <c r="K63" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M63" s="26"/>
@@ -3345,175 +3457,195 @@
       <c r="S63" t="n">
         <v>103.0</v>
       </c>
-      <c r="T63" t="n" s="37">
+      <c r="T63" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" s="22"/>
-      <c r="C64" t="s" s="151">
+      <c r="C64" t="s" s="150">
         <v>3</v>
       </c>
       <c r="D64" s="26"/>
-      <c r="K64" s="37"/>
+      <c r="K64" s="38"/>
       <c r="M64" t="s" s="30">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>115</v>
+        <v>118</v>
+      </c>
+      <c r="O64" t="s" s="2">
+        <v>6</v>
       </c>
       <c r="R64" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="T64" s="37"/>
+        <v>119</v>
+      </c>
+      <c r="T64" s="38"/>
     </row>
     <row r="65">
       <c r="B65" s="22"/>
-      <c r="C65" t="s" s="152">
-        <v>10</v>
+      <c r="C65" t="s" s="151">
+        <v>11</v>
       </c>
       <c r="D65" s="26"/>
-      <c r="K65" s="37"/>
-      <c r="M65" t="s" s="46">
-        <v>117</v>
+      <c r="K65" s="38"/>
+      <c r="M65" t="s" s="32">
+        <v>120</v>
       </c>
       <c r="N65" t="s" s="3">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="O65" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="P65" t="s" s="3">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="Q65" t="s" s="3">
-        <v>120</v>
-      </c>
-      <c r="T65" s="37"/>
+        <v>123</v>
+      </c>
+      <c r="T65" s="38"/>
     </row>
     <row r="66">
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
       <c r="D66" s="26"/>
-      <c r="K66" s="37"/>
-      <c r="M66" t="s" s="46">
-        <v>121</v>
+      <c r="K66" s="38"/>
+      <c r="M66" t="s" s="32">
+        <v>124</v>
       </c>
       <c r="N66" t="s" s="3">
-        <v>122</v>
-      </c>
-      <c r="P66" t="s" s="3">
-        <v>123</v>
+        <v>125</v>
+      </c>
+      <c r="O66" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="Q66" t="s" s="3">
-        <v>124</v>
-      </c>
-      <c r="T66" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="T66" s="38"/>
     </row>
     <row r="67">
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
       <c r="D67" s="26"/>
-      <c r="K67" s="37"/>
-      <c r="M67" t="s" s="46">
-        <v>125</v>
+      <c r="K67" s="38"/>
+      <c r="M67" t="s" s="32">
+        <v>127</v>
       </c>
       <c r="N67" t="s" s="3">
-        <v>126</v>
+        <v>128</v>
+      </c>
+      <c r="O67" t="s" s="3">
+        <v>6</v>
+      </c>
+      <c r="P67" t="s" s="3">
+        <v>129</v>
       </c>
       <c r="Q67" t="s" s="3">
-        <v>127</v>
-      </c>
-      <c r="T67" s="37"/>
+        <v>130</v>
+      </c>
+      <c r="T67" s="38"/>
     </row>
     <row r="68">
       <c r="B68" s="22"/>
-      <c r="C68" t="s" s="154">
-        <v>48</v>
+      <c r="C68" t="s" s="153">
+        <v>52</v>
       </c>
       <c r="D68" s="26"/>
-      <c r="K68" s="37"/>
-      <c r="M68" t="s" s="160">
-        <v>128</v>
+      <c r="K68" s="38"/>
+      <c r="M68" t="s" s="159">
+        <v>131</v>
       </c>
       <c r="N68" t="s" s="7">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="O68" t="s" s="7">
+        <v>6</v>
       </c>
       <c r="P68" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="T68" s="37"/>
+        <v>62</v>
+      </c>
+      <c r="T68" s="38"/>
     </row>
     <row r="69">
       <c r="B69" s="22"/>
-      <c r="C69" t="s" s="155">
-        <v>12</v>
+      <c r="C69" t="s" s="154">
+        <v>16</v>
       </c>
       <c r="D69" s="26"/>
-      <c r="K69" s="37"/>
-      <c r="M69" t="s" s="69">
-        <v>130</v>
+      <c r="K69" s="38"/>
+      <c r="M69" t="s" s="48">
+        <v>133</v>
       </c>
       <c r="N69" t="s" s="9">
-        <v>131</v>
+        <v>134</v>
+      </c>
+      <c r="O69" t="s" s="9">
+        <v>6</v>
       </c>
       <c r="P69" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="T69" s="37"/>
+        <v>135</v>
+      </c>
+      <c r="T69" s="38"/>
     </row>
     <row r="70">
-      <c r="B70" s="32"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="38"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="38"/>
-      <c r="J70" s="38"/>
-      <c r="K70" s="40"/>
-      <c r="M70" t="s" s="48">
-        <v>132</v>
-      </c>
-      <c r="N70" t="s" s="49">
-        <v>133</v>
-      </c>
-      <c r="O70" s="38"/>
-      <c r="P70" t="s" s="49">
-        <v>134</v>
-      </c>
-      <c r="Q70" s="38"/>
-      <c r="R70" s="38"/>
-      <c r="S70" s="38"/>
-      <c r="T70" s="40"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="41"/>
+      <c r="M70" t="s" s="49">
+        <v>136</v>
+      </c>
+      <c r="N70" t="s" s="50">
+        <v>137</v>
+      </c>
+      <c r="O70" t="s" s="50">
+        <v>6</v>
+      </c>
+      <c r="P70" t="s" s="50">
+        <v>51</v>
+      </c>
+      <c r="Q70" s="39"/>
+      <c r="R70" s="39"/>
+      <c r="S70" s="39"/>
+      <c r="T70" s="41"/>
     </row>
     <row r="72">
       <c r="B72" t="s" s="21">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C72" s="23"/>
-      <c r="D72" t="s" s="166">
+      <c r="D72" t="s" s="165">
         <v>0</v>
       </c>
       <c r="E72" s="25"/>
       <c r="F72" s="25"/>
-      <c r="G72" t="s" s="169">
+      <c r="G72" t="s" s="168">
         <v>1</v>
       </c>
       <c r="H72" s="25"/>
       <c r="I72" s="25"/>
       <c r="J72" s="25"/>
-      <c r="K72" s="34"/>
-      <c r="M72" t="s" s="172">
-        <v>14</v>
+      <c r="K72" s="36"/>
+      <c r="M72" t="s" s="171">
+        <v>18</v>
       </c>
       <c r="N72" s="25"/>
       <c r="O72" s="25"/>
-      <c r="P72" t="s" s="173">
+      <c r="P72" t="s" s="172">
         <v>1</v>
       </c>
       <c r="Q72" s="25"/>
       <c r="R72" s="25"/>
       <c r="S72" s="25"/>
-      <c r="T72" s="34"/>
+      <c r="T72" s="36"/>
     </row>
     <row r="73">
       <c r="B73" s="22"/>
@@ -3531,7 +3663,7 @@
       <c r="J73" t="n">
         <v>103.0</v>
       </c>
-      <c r="K73" t="n" s="37">
+      <c r="K73" t="n" s="38">
         <v>104.0</v>
       </c>
       <c r="M73" s="26"/>
@@ -3547,72 +3679,78 @@
       <c r="S73" t="n">
         <v>103.0</v>
       </c>
-      <c r="T73" t="n" s="37">
+      <c r="T73" t="n" s="38">
         <v>104.0</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" s="22"/>
-      <c r="C74" t="s" s="167">
-        <v>10</v>
+      <c r="C74" t="s" s="166">
+        <v>11</v>
       </c>
       <c r="D74" s="26"/>
-      <c r="K74" s="37"/>
-      <c r="M74" t="s" s="46">
-        <v>135</v>
+      <c r="K74" s="38"/>
+      <c r="M74" t="s" s="32">
+        <v>138</v>
       </c>
       <c r="N74" t="s" s="3">
-        <v>136</v>
+        <v>139</v>
+      </c>
+      <c r="O74" t="s" s="3">
+        <v>6</v>
       </c>
       <c r="P74" t="s" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q74" t="s" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R74" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S74" t="s" s="3">
-        <v>137</v>
-      </c>
-      <c r="T74" s="37"/>
+        <v>140</v>
+      </c>
+      <c r="T74" s="38"/>
     </row>
     <row r="75">
-      <c r="B75" s="32"/>
-      <c r="C75" t="s" s="168">
-        <v>11</v>
-      </c>
-      <c r="D75" s="36"/>
-      <c r="E75" s="38"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="38"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="40"/>
-      <c r="M75" t="s" s="174">
-        <v>138</v>
-      </c>
-      <c r="N75" t="s" s="175">
-        <v>139</v>
-      </c>
-      <c r="O75" s="38"/>
-      <c r="P75" t="s" s="175">
-        <v>29</v>
-      </c>
-      <c r="Q75" t="s" s="175">
-        <v>89</v>
-      </c>
-      <c r="R75" s="38"/>
-      <c r="S75" s="38"/>
-      <c r="T75" s="40"/>
+      <c r="B75" s="34"/>
+      <c r="C75" t="s" s="167">
+        <v>15</v>
+      </c>
+      <c r="D75" s="37"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="39"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="41"/>
+      <c r="M75" t="s" s="173">
+        <v>141</v>
+      </c>
+      <c r="N75" t="s" s="174">
+        <v>142</v>
+      </c>
+      <c r="O75" t="s" s="174">
+        <v>6</v>
+      </c>
+      <c r="P75" t="s" s="174">
+        <v>30</v>
+      </c>
+      <c r="Q75" t="s" s="174">
+        <v>93</v>
+      </c>
+      <c r="R75" s="39"/>
+      <c r="S75" s="39"/>
+      <c r="T75" s="41"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="D11:F12"/>
     <mergeCell ref="G11:K11"/>
-    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="B11:B19"/>
     <mergeCell ref="M11:O12"/>
     <mergeCell ref="P11:T11"/>

</xml_diff>